<commit_message>
Diverse wijzigingen in datamodel aangebracht
</commit_message>
<xml_diff>
--- a/NVWA DTV/Autorisaties.xlsx
+++ b/NVWA DTV/Autorisaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="528" windowWidth="16956" windowHeight="7356" firstSheet="11" activeTab="17"/>
+    <workbookView xWindow="132" yWindow="528" windowWidth="16956" windowHeight="7356" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Akkoord" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>Akkoord</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Functie</t>
   </si>
   <si>
-    <t>Initialen</t>
-  </si>
-  <si>
     <t>Loginnaam</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>Telefoonnummer</t>
-  </si>
-  <si>
     <t>TijdRubriekCategorie</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>Tijdverantwoording</t>
   </si>
   <si>
-    <t>Titel</t>
-  </si>
-  <si>
     <t>Verantwoordingsperiode</t>
   </si>
   <si>
@@ -217,9 +208,6 @@
     <t>functie</t>
   </si>
   <si>
-    <t>geboortedatum</t>
-  </si>
-  <si>
     <t>geldigTot</t>
   </si>
   <si>
@@ -238,9 +226,6 @@
     <t>ingelogd~</t>
   </si>
   <si>
-    <t>initialen</t>
-  </si>
-  <si>
     <t>leidinggevende</t>
   </si>
   <si>
@@ -271,9 +256,6 @@
     <t>periodeverantwoording</t>
   </si>
   <si>
-    <t>persoonsnaam</t>
-  </si>
-  <si>
     <t>persoonsnr</t>
   </si>
   <si>
@@ -295,9 +277,6 @@
     <t>team</t>
   </si>
   <si>
-    <t>telefoon</t>
-  </si>
-  <si>
     <t>tijdCategorie</t>
   </si>
   <si>
@@ -305,9 +284,6 @@
   </si>
   <si>
     <t>tijdsduur</t>
-  </si>
-  <si>
-    <t>titel</t>
   </si>
   <si>
     <t>toelichting</t>
@@ -672,32 +648,235 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -707,233 +886,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -941,15 +917,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -967,10 +943,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -996,22 +972,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1031,7 +1007,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1059,22 +1035,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1082,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1091,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1109,25 +1085,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1135,16 +1111,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1168,36 +1144,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1209,124 +1185,96 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1346,57 +1294,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -1405,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1423,10 +1371,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1434,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change Persoon -> Account make 2 versions of comments for Login.adl
</commit_message>
<xml_diff>
--- a/NVWA DTV/Autorisaties.xlsx
+++ b/NVWA DTV/Autorisaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="528" windowWidth="16956" windowHeight="7356" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="135" yWindow="525" windowWidth="16950" windowHeight="7350" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Akkoord" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="persoonsnr" sheetId="18" r:id="rId18"/>
     <sheet name="tijdCategorie" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -91,9 +91,6 @@
     <t>Personeelsnummer</t>
   </si>
   <si>
-    <t>Persoon</t>
-  </si>
-  <si>
     <t>SESSION</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>[Personeelsnummer]</t>
   </si>
   <si>
-    <t>[Persoon]</t>
-  </si>
-  <si>
     <t>[SESSION]</t>
   </si>
   <si>
@@ -302,6 +296,12 @@
   </si>
   <si>
     <t>wachtwoord</t>
+  </si>
+  <si>
+    <t>[Account]</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
 </sst>
 </file>
@@ -341,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -354,9 +354,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -394,7 +394,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -466,7 +466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -644,17 +644,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -679,14 +679,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -694,6 +694,180 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -702,202 +876,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -913,14 +913,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -939,14 +939,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -968,26 +968,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
       </c>
       <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1023,34 +1023,34 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,29 +1081,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1117,10 +1117,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1140,32 +1140,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1185,7 +1185,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1203,29 +1203,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
       </c>
       <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1234,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1248,22 +1246,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1274,7 +1272,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1290,61 +1288,61 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -1353,7 +1351,7 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1367,14 +1365,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>